<commit_message>
cleaned the data to get weeks of season
</commit_message>
<xml_diff>
--- a/data/atlanta.xlsx
+++ b/data/atlanta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clint\Documents\nss\Capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EF0F8F-65BC-4F79-81B3-06DB3F1596B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26E0925-BE07-47AC-B7D6-BC17E2F09DB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11580" activeTab="9" xr2:uid="{7F84BC0D-6CA1-4BFA-B25A-BA34220402DF}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{7F84BC0D-6CA1-4BFA-B25A-BA34220402DF}"/>
   </bookViews>
   <sheets>
     <sheet name="2011" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2340" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="368">
   <si>
     <t>Player </t>
   </si>
@@ -1047,9 +1047,6 @@
     <t>Luke Stocker</t>
   </si>
   <si>
-    <t>J.J. Wilcox</t>
-  </si>
-  <si>
     <t>Matt Wile</t>
   </si>
   <si>
@@ -1126,6 +1123,21 @@
   </si>
   <si>
     <t>Olamide Zaccheaus</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>RaShede Hageman</t>
+  </si>
+  <si>
+    <t>JJ Wilcox</t>
+  </si>
+  <si>
+    <t>Blidi Wreh Wilson</t>
+  </si>
+  <si>
+    <t>12/20vs. TAM</t>
   </si>
 </sst>
 </file>
@@ -2325,59 +2337,65 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F73A358-C8CC-4321-9FA0-DC5607F33735}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>363</v>
       </c>
       <c r="B1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C1" t="s">
         <v>339</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>340</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>341</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>342</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>343</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>344</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>345</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>346</v>
-      </c>
-      <c r="J1" t="s">
-        <v>347</v>
       </c>
       <c r="K1" t="s">
         <v>282</v>
       </c>
       <c r="L1" t="s">
+        <v>347</v>
+      </c>
+      <c r="M1" t="s">
         <v>348</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>349</v>
       </c>
-      <c r="N1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>178</v>
       </c>
@@ -2388,26 +2406,26 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>323</v>
       </c>
       <c r="G3" t="s">
+        <v>350</v>
+      </c>
+      <c r="H3" t="s">
+        <v>350</v>
+      </c>
+      <c r="I3" t="s">
+        <v>350</v>
+      </c>
+      <c r="J3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
         <v>351</v>
-      </c>
-      <c r="H3" t="s">
-        <v>351</v>
-      </c>
-      <c r="I3" t="s">
-        <v>351</v>
-      </c>
-      <c r="J3" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>352</v>
       </c>
       <c r="B4" t="s">
         <v>48</v>
@@ -2416,94 +2434,94 @@
         <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I4" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.75">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
+        <v>352</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
         <v>353</v>
       </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" t="s">
+        <v>350</v>
+      </c>
+      <c r="L6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
         <v>354</v>
       </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" t="s">
-        <v>351</v>
-      </c>
-      <c r="L6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
+      <c r="L7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
         <v>355</v>
       </c>
-      <c r="L7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
         <v>356</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
         <v>357</v>
       </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
-        <v>358</v>
-      </c>
       <c r="L10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -2520,7 +2538,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>327</v>
       </c>
@@ -2551,16 +2569,19 @@
       <c r="N12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -2568,15 +2589,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>293</v>
       </c>
@@ -2599,9 +2620,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J17" t="s">
         <v>35</v>
@@ -2618,8 +2639,11 @@
       <c r="N17" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>234</v>
       </c>
@@ -2627,15 +2651,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>333</v>
       </c>
@@ -2646,7 +2670,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>334</v>
       </c>
@@ -2660,9 +2684,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L22" t="s">
         <v>35</v>
@@ -2671,6 +2695,9 @@
         <v>35</v>
       </c>
       <c r="N22" t="s">
+        <v>35</v>
+      </c>
+      <c r="O22" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5650,6 +5677,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
@@ -6554,6 +6584,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="15.2265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
@@ -7301,14 +7334,17 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="29.1328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>363</v>
       </c>
       <c r="B1" t="s">
         <v>240</v>
@@ -8331,14 +8367,17 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="32.04296875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>363</v>
       </c>
       <c r="B1" t="s">
         <v>299</v>
@@ -8831,7 +8870,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>364</v>
       </c>
       <c r="D18" t="s">
         <v>35</v>
@@ -9274,7 +9313,7 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A40" t="s">
-        <v>337</v>
+        <v>365</v>
       </c>
       <c r="B40" t="s">
         <v>35</v>
@@ -9327,7 +9366,7 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A41" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G41" t="s">
         <v>20</v>
@@ -9335,7 +9374,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A42" t="s">
-        <v>298</v>
+        <v>366</v>
       </c>
       <c r="F42" t="s">
         <v>20</v>

</xml_diff>